<commit_message>
Too Many Mods - Compats and Rebalances 업데이트
</commit_message>
<xml_diff>
--- a/Data/Too Many Mods - Compats and Rebalances - 3250762483/3250762483.xlsx
+++ b/Data/Too Many Mods - Compats and Rebalances - 3250762483/3250762483.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.9.1\result (11)\림월드 번역\Too Many Mods - Compats and Rebalances - 3250762483\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\OneDrive\바탕 화면\림월드 번역\림월드 번역\Too Many Mods - Compats and Rebalances - 3250762483\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAEAEF4-BDFF-46A3-AB44-FAC168DCC428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719D0398-7F19-4055-A377-D221F8A9D856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240707" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,479 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>bjmi0</author>
+  </authors>
+  <commentList>
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-07-11</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>에</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>삭제됨</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>삭제</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>이전</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>번역문</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>: '</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>드워프주의</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-07-11</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>에</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>삭제됨</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>삭제</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>이전</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>번역문</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>: '</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>키</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>작은</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>이들로부터</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>이어진</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>드워프주의</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>체제입니다</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-07-11</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>에</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>새로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>추가된</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>노드들</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (8</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+          </rPr>
+          <t>개</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-07-19에 새로 추가된 노드들 (1개)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{51270131-96E7-4A08-917B-71472188EBCB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-07-19에 새로 추가된 노드들 (1개)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="82">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -52,6 +523,18 @@
     <t>toomanymods: uncheck this to enable basic removals</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>toomanymods: 기본적으로 제거된 것들을 되돌리려면 이 옵션을 비활성화하세요.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>PawnKindDef+Empire_Fighter_Cataphract_Hussar.label</t>
   </si>
   <si>
@@ -64,6 +547,18 @@
     <t>cataphract</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>철갑기병</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Keyed+MeditationFocusPerSuperComputerAbstract</t>
   </si>
   <si>
@@ -76,6 +571,18 @@
     <t>{1} per nearby supercomputer (max {0})</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>근처의 슈퍼컴퓨터당 {1} (최대 {0})</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Keyed+MeditationFocusPerSuperComputer</t>
   </si>
   <si>
@@ -85,6 +592,18 @@
     <t>{2} per nearby supercomputer ({0} / {1})</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>근처의 슈퍼컴퓨터당 {2} ({0} / {1})</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Keyed+MeditationFocusPerWealthyAbstract</t>
   </si>
   <si>
@@ -94,6 +613,18 @@
     <t>2-6% per nearby wealthy building (max {0})</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>근처의 부유한 건물당 2-6% (최대 {0})</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Keyed+MeditationFocusPerWealthy</t>
   </si>
   <si>
@@ -103,6 +634,18 @@
     <t>2-6% per nearby wealthy building ({0} / {1})</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>근처의 부유한 건물당 2-6% ({0} / {1})</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Keyed+VFEP.ActivateShieldDescNerfed</t>
   </si>
   <si>
@@ -112,71 +655,241 @@
     <t>Click to activate the shield field. It has 5 seconds of active mode and then 90 seconds cooldown.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>보호막 영역을 활성화합니다. 5초 동안 지속되며 90초의 재사용 대기시간이 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>CultureDef+TMM_Dwarven.label</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>CultureDef</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>TMM_Dwarven.label</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Stoneborn - Dwarven Style Pack &amp;&amp; Det's Xenotypes - Stoneborn</t>
   </si>
   <si>
     <t>dwarven</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>패치 ㄴㄴ</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>CultureDef+TMM_Dwarven.description</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>TMM_Dwarven.description</t>
   </si>
   <si>
     <t>A hardy dwarven culture common among small people.</t>
   </si>
   <si>
-    <t>toomanymods: 기본적으로 제거된 것들을 되돌리려면 이 옵션을 비활성화하세요.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>Keyed+VCE_CondimentEffects</t>
+  </si>
+  <si>
+    <t>VCE_CondimentEffects</t>
+  </si>
+  <si>
+    <t>Condiment effects</t>
+  </si>
+  <si>
+    <t>Keyed+TMM_VCE_CondimentEffectsLuciferiumPowder</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>조미료 효과</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>TMM_VCE_CondimentEffectsLuciferiumPowder</t>
+  </si>
+  <si>
+    <t>Consuming meals that include this condiment increases sight, blood pumping and filtration by 5%, increases consciousness, moving, breathing and digestion by 2%, and reduces pain by 5% for 12 hours.</t>
+  </si>
+  <si>
+    <t>Keyed+TMM_VCE_CondimentEffectsWakeUpPowder</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>이 조미료가 포함된 식사를 섭취하면 12시간 동안 시력, 혈액 펌프 및 여과 기능이 5% 향상되고 의식, 움직임, 호흡 및 소화가 2% 증가하며 통증이 5% 감소합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>TMM_VCE_CondimentEffectsWakeUpPowder</t>
+  </si>
+  <si>
+    <t>Consuming meals that include this condiment increases global work speed by 10%, increases meditation psyfocus gain by 5%, increases consciousness and moving by 3%, and reduces tiredness by 5% for 12 hours.</t>
+  </si>
+  <si>
+    <t>이 조미료가 포함된 식사를 섭취하면 12시간 동안 전역 작업 속도가 10% 증가하고, 명상 정신 집중력이 5% 증가하며, 의식과 움직임이 3% 증가하고, 피로가 5% 감소합니다.</t>
+  </si>
+  <si>
+    <t>Keyed+TMM_VCE_CondimentEffectsGoJuiceStock</t>
+  </si>
+  <si>
+    <t>TMM_VCE_CondimentEffectsGoJuiceStock</t>
+  </si>
+  <si>
+    <t>Consuming meals that include this condiment increases sight and moving by 5%, increases consciousness by 3%, and reduces pain by 10% for 12 hours.</t>
+  </si>
+  <si>
+    <t>Patches.CultureDef+TMM_Draconic.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>이 조미료가 포함된 식사를 섭취하면 12시간 동안 시력과 움직임이 5% 증가하고, 의식이 3% 증가하며, 통증이 10% 감소합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patches.CultureDef</t>
+  </si>
+  <si>
+    <t>TMM_Draconic.label</t>
+  </si>
+  <si>
+    <t>Biotech Expansion - Mammalia &amp;&amp; ATH's style Draconic</t>
+  </si>
+  <si>
+    <t>draconic</t>
+  </si>
+  <si>
+    <t>Patches.CultureDef+TMM_Draconic.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>드래곤주의</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>TMM_Draconic.description</t>
+  </si>
+  <si>
+    <t>A draconic culture among rimworld tribes led by mythical xenohumans.</t>
+  </si>
+  <si>
+    <t>Patches.CultureDef+TMM_Dwarven.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>신화 속 이질적인 인간들이 이끄는 드래곤의 문화입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>TMM_Dwarven.label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stoneborn - Dwarven Style Pack &amp;&amp;  (( Det's Xenotypes - Stoneborn || Big and Small - Races )) </t>
   </si>
   <si>
     <t>드워프주의</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patches.CultureDef+TMM_Dwarven.description</t>
   </si>
   <si>
     <t>키 작은 이들로부터 이어진 드워프주의 체제입니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>보호막 영역을 활성화합니다. 5초 동안 지속되며 90초의 재사용 대기시간이 있습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>근처의 슈퍼컴퓨터당 {1} (최대 {0})</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>근처의 슈퍼컴퓨터당 {2} ({0} / {1})</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>근처의 부유한 건물당 2-6% (최대 {0})</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>근처의 부유한 건물당 2-6% ({0} / {1})</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>철갑기병</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TMM_Dwarven.label</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CultureDef</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CultureDef+TMM_Dwarven.label</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CultureDef+TMM_Dwarven.description</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>패치 ㄴㄴ</t>
+  </si>
+  <si>
+    <t>CherryPicker.DefList+TMM_CherryPicker_All.label</t>
+  </si>
+  <si>
+    <t>TMM_CherryPicker_All.label</t>
+  </si>
+  <si>
+    <t>toomanymods: uncheck then re-check this to revive everything</t>
+  </si>
+  <si>
+    <t>toomanymods: 선택을 취소했다가 다시 선택하면 모든 항목이 다시 활성화됩니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -184,7 +897,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -204,13 +917,19 @@
       <charset val="129"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="돋움체"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +939,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87CEEB"/>
       </patternFill>
     </fill>
   </fills>
@@ -247,19 +976,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="메모" xfId="1" builtinId="10"/>
+  <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -559,11 +1286,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -612,159 +1339,319 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>47</v>
+      <c r="D19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>